<commit_message>
fix(data): add real ids
</commit_message>
<xml_diff>
--- a/RoomData.xlsx
+++ b/RoomData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>CoverPicture</t>
+  </si>
+  <si>
+    <t>0195e7a9-181c-728b-bc78-0a90c0cd8d0f</t>
   </si>
   <si>
     <t xml:space="preserve">Frontend Bootcamp</t>
@@ -204,10 +207,13 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0"/>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="0" pivotButton="0">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0">
+      <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0">
       <protection hidden="0" locked="1"/>
@@ -741,6 +747,7 @@
     <col customWidth="1" min="3" max="3" width="31.140625"/>
     <col customWidth="1" min="4" max="4" width="39.7109375"/>
     <col customWidth="1" min="7" max="7" width="33.28125"/>
+    <col bestFit="1" min="9" max="9" width="14.8125"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -779,276 +786,276 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2">
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3">
         <v>101</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3">
+      <c r="H2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="4">
         <v>45778.416666666664</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="3">
         <v>15</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>102</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="4">
+        <v>24</v>
+      </c>
+      <c r="I3" s="5">
         <v>45787.395833333336</v>
       </c>
       <c r="J3">
         <v>20</v>
       </c>
       <c r="K3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4">
         <v>103</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="4">
+        <v>30</v>
+      </c>
+      <c r="I4" s="5">
         <v>45792.510416666664</v>
       </c>
       <c r="J4">
         <v>12</v>
       </c>
       <c r="K4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5">
-        <v>4</v>
+      <c r="A5" t="s">
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5">
         <v>104</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="4">
+        <v>37</v>
+      </c>
+      <c r="I5" s="5">
         <v>45797.614583333336</v>
       </c>
       <c r="J5">
         <v>8</v>
       </c>
       <c r="K5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="3">
         <v>105</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="3">
+      <c r="H6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="4">
         <v>45802.458333333336</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="3">
         <v>10</v>
       </c>
       <c r="K6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="C11" s="2"/>
+      <c r="C11" s="3"/>
     </row>
     <row r="12" ht="14.25">
-      <c r="C12" s="2"/>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" ht="14.25">
-      <c r="C13" s="2"/>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" ht="14.25">
-      <c r="C14" s="2"/>
+      <c r="C14" s="3"/>
     </row>
     <row r="15" ht="14.25">
-      <c r="C15" s="2"/>
+      <c r="C15" s="3"/>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>